<commit_message>
stop create report to update code for caculation lasary
</commit_message>
<xml_diff>
--- a/notion_data/CHAM_CONG_HE_THONG.xlsx
+++ b/notion_data/CHAM_CONG_HE_THONG.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ14"/>
+  <dimension ref="A1:AQ20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -658,17 +658,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0f6b9d94-3550-435e-9360-d1dd8933363f</t>
+          <t>44a59162-be99-4049-96cd-2374839aa086</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-07-06T10:33:00.000Z</t>
+          <t>2024-07-08T16:49:00.000Z</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-07-08T01:58:00.000Z</t>
+          <t>2024-07-17T12:15:00.000Z</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -681,7 +681,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>https://www.notion.so/0f6b9d943550435e9360d1dd8933363f</t>
+          <t>https://www.notion.so/44a59162be99404996cd2374839aa086</t>
         </is>
       </c>
       <c r="J2" t="inlineStr"/>
@@ -753,7 +753,7 @@
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>[{'id': 'd8178da7-a5cc-474f-9c6e-ed3029f89c4d'}]</t>
+          <t>[{'id': 'ea0572af-f8c9-430d-9d95-23303a4ce4cd'}]</t>
         </is>
       </c>
       <c r="Z2" t="b">
@@ -770,7 +770,7 @@
         </is>
       </c>
       <c r="AC2" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="AD2" t="inlineStr">
         <is>
@@ -783,7 +783,7 @@
         </is>
       </c>
       <c r="AF2" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="AG2" t="inlineStr">
         <is>
@@ -796,7 +796,7 @@
         </is>
       </c>
       <c r="AI2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ2" t="inlineStr">
         <is>
@@ -815,7 +815,7 @@
       </c>
       <c r="AM2" t="inlineStr">
         <is>
-          <t>[{'type': 'select', 'select': {'id': 'Lj_l', 'name': 'LONG XUYÊN', 'color': 'green'}}]</t>
+          <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
         </is>
       </c>
       <c r="AN2" t="inlineStr">
@@ -847,17 +847,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>05de003a-828f-46b1-ba9c-63df15fb2410</t>
+          <t>39c98d7f-b7d0-49ef-9652-f406a3e62029</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2024-07-02T18:08:00.000Z</t>
+          <t>2024-07-08T16:48:00.000Z</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2024-07-08T01:58:00.000Z</t>
+          <t>2024-07-17T12:15:00.000Z</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -870,7 +870,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>https://www.notion.so/05de003a828f46b1ba9c63df15fb2410</t>
+          <t>https://www.notion.so/39c98d7fb7d049ef9652f406a3e62029</t>
         </is>
       </c>
       <c r="J3" t="inlineStr"/>
@@ -942,7 +942,7 @@
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>[{'id': 'f973382b-037a-4eb1-84bc-e9e5318184b8'}]</t>
+          <t>[{'id': 'e0ac0375-0b3a-4c88-a613-cb8df33ebe6b'}]</t>
         </is>
       </c>
       <c r="Z3" t="b">
@@ -959,7 +959,7 @@
         </is>
       </c>
       <c r="AC3" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="AD3" t="inlineStr">
         <is>
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="AF3" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="AG3" t="inlineStr">
         <is>
@@ -1036,17 +1036,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1cf1ba2b-e08a-4452-b208-684506d74f54</t>
+          <t>4a76f2d2-b0f3-4746-8b60-6095030ce9a4</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2024-07-02T18:08:00.000Z</t>
+          <t>2024-07-08T16:48:00.000Z</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2024-07-08T01:58:00.000Z</t>
+          <t>2024-07-17T12:15:00.000Z</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>https://www.notion.so/1cf1ba2be08a4452b208684506d74f54</t>
+          <t>https://www.notion.so/4a76f2d2b0f347468b606095030ce9a4</t>
         </is>
       </c>
       <c r="J4" t="inlineStr"/>
@@ -1131,7 +1131,7 @@
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>[{'id': '3fac4a49-402c-4d34-aa91-419ebc20760c'}]</t>
+          <t>[{'id': '90bc02c2-bd1e-4c33-884a-38a1db528c78'}]</t>
         </is>
       </c>
       <c r="Z4" t="b">
@@ -1148,7 +1148,7 @@
         </is>
       </c>
       <c r="AC4" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AD4" t="inlineStr">
         <is>
@@ -1161,7 +1161,7 @@
         </is>
       </c>
       <c r="AF4" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AG4" t="inlineStr">
         <is>
@@ -1225,17 +1225,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>dda0b264-3b1d-46ab-85d8-06a4ac6fc467</t>
+          <t>8e8f7e77-65ea-4667-9635-359ff100cf58</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2024-07-02T18:08:00.000Z</t>
+          <t>2024-07-08T16:47:00.000Z</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2024-07-08T01:58:00.000Z</t>
+          <t>2024-07-17T12:15:00.000Z</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>https://www.notion.so/dda0b2643b1d46ab85d806a4ac6fc467</t>
+          <t>https://www.notion.so/8e8f7e7765ea46679635359ff100cf58</t>
         </is>
       </c>
       <c r="J5" t="inlineStr"/>
@@ -1293,7 +1293,7 @@
         </is>
       </c>
       <c r="S5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T5" t="inlineStr">
         <is>
@@ -1320,7 +1320,7 @@
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>[{'id': '75046948-a198-4627-89b3-3bbf5967526b'}]</t>
+          <t>[{'id': '6454d5e5-8a20-473b-a597-dc1973dd1e0e'}]</t>
         </is>
       </c>
       <c r="Z5" t="b">
@@ -1337,7 +1337,7 @@
         </is>
       </c>
       <c r="AC5" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AD5" t="inlineStr">
         <is>
@@ -1350,7 +1350,7 @@
         </is>
       </c>
       <c r="AF5" t="n">
-        <v>6.5</v>
+        <v>0</v>
       </c>
       <c r="AG5" t="inlineStr">
         <is>
@@ -1382,7 +1382,7 @@
       </c>
       <c r="AM5" t="inlineStr">
         <is>
-          <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
+          <t>[{'type': 'select', 'select': {'id': 'VWB;', 'name': 'SÓC TRĂNG', 'color': 'red'}}]</t>
         </is>
       </c>
       <c r="AN5" t="inlineStr">
@@ -1414,17 +1414,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>36015951-56f5-48c6-b457-456fdded4f32</t>
+          <t>0326afbb-4995-4ae7-8b30-901ef3dd038c</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2024-07-02T18:08:00.000Z</t>
+          <t>2024-07-08T16:45:00.000Z</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2024-07-08T01:58:00.000Z</t>
+          <t>2024-07-17T12:15:00.000Z</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>https://www.notion.so/3601595156f548c6b457456fdded4f32</t>
+          <t>https://www.notion.so/0326afbb49954ae78b30901ef3dd038c</t>
         </is>
       </c>
       <c r="J6" t="inlineStr"/>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>[{'id': 'e49d0ce3-124d-4e4b-b377-be2139cde3f5'}]</t>
+          <t>[{'id': 'bc9b2b6b-3140-44b9-a1be-4dc8e77d8898'}]</t>
         </is>
       </c>
       <c r="Z6" t="b">
@@ -1526,7 +1526,7 @@
         </is>
       </c>
       <c r="AC6" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="AD6" t="inlineStr">
         <is>
@@ -1539,7 +1539,7 @@
         </is>
       </c>
       <c r="AF6" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="AG6" t="inlineStr">
         <is>
@@ -1552,7 +1552,7 @@
         </is>
       </c>
       <c r="AI6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ6" t="inlineStr">
         <is>
@@ -1603,17 +1603,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>48a1d5d5-449f-4119-b338-1f7d4ea3464f</t>
+          <t>8170c5f7-1afc-4ec2-b5bf-4dfa06dfd8a8</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2024-07-02T18:08:00.000Z</t>
+          <t>2024-07-08T16:45:00.000Z</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2024-07-08T01:58:00.000Z</t>
+          <t>2024-07-17T12:15:00.000Z</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>https://www.notion.so/48a1d5d5449f4119b3381f7d4ea3464f</t>
+          <t>https://www.notion.so/8170c5f71afc4ec2b5bf4dfa06dfd8a8</t>
         </is>
       </c>
       <c r="J7" t="inlineStr"/>
@@ -1698,7 +1698,7 @@
       </c>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>[{'id': 'c463b1a9-4fb2-4258-87a7-44193ba02405'}]</t>
+          <t>[{'id': '7e29a9ca-b017-4ad6-a6b0-6ed9330137bc'}]</t>
         </is>
       </c>
       <c r="Z7" t="b">
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="AC7" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AD7" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
         </is>
       </c>
       <c r="AF7" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AG7" t="inlineStr">
         <is>
@@ -1760,7 +1760,7 @@
       </c>
       <c r="AM7" t="inlineStr">
         <is>
-          <t>[{'type': 'select', 'select': {'id': 'VWB;', 'name': 'SÓC TRĂNG', 'color': 'red'}}]</t>
+          <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
         </is>
       </c>
       <c r="AN7" t="inlineStr">
@@ -1792,17 +1792,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>4a2d1406-11a9-4e3c-80ff-0b01e9355c9b</t>
+          <t>0f6b9d94-3550-435e-9360-d1dd8933363f</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2024-07-02T18:08:00.000Z</t>
+          <t>2024-07-06T10:33:00.000Z</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2024-07-08T01:58:00.000Z</t>
+          <t>2024-07-17T12:15:00.000Z</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>https://www.notion.so/4a2d140611a94e3c80ff0b01e9355c9b</t>
+          <t>https://www.notion.so/0f6b9d943550435e9360d1dd8933363f</t>
         </is>
       </c>
       <c r="J8" t="inlineStr"/>
@@ -1860,77 +1860,77 @@
         </is>
       </c>
       <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>%3CK%3FH</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="V8" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>Kfrh</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>relation</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>[{'id': 'd8178da7-a5cc-474f-9c6e-ed3029f89c4d'}]</t>
+        </is>
+      </c>
+      <c r="Z8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>avzr</t>
+        </is>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AC8" t="n">
+        <v>16</v>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t>rCIq</t>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AF8" t="n">
+        <v>17</v>
+      </c>
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t>%7B%3EFf</t>
+        </is>
+      </c>
+      <c r="AH8" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AI8" t="n">
         <v>1</v>
-      </c>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>%3CK%3FH</t>
-        </is>
-      </c>
-      <c r="U8" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="V8" t="n">
-        <v>0</v>
-      </c>
-      <c r="W8" t="inlineStr">
-        <is>
-          <t>Kfrh</t>
-        </is>
-      </c>
-      <c r="X8" t="inlineStr">
-        <is>
-          <t>relation</t>
-        </is>
-      </c>
-      <c r="Y8" t="inlineStr">
-        <is>
-          <t>[{'id': 'e926d62c-e624-4663-9009-c562ae5166cf'}]</t>
-        </is>
-      </c>
-      <c r="Z8" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA8" t="inlineStr">
-        <is>
-          <t>avzr</t>
-        </is>
-      </c>
-      <c r="AB8" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="AC8" t="n">
-        <v>6</v>
-      </c>
-      <c r="AD8" t="inlineStr">
-        <is>
-          <t>rCIq</t>
-        </is>
-      </c>
-      <c r="AE8" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="AF8" t="n">
-        <v>6.5</v>
-      </c>
-      <c r="AG8" t="inlineStr">
-        <is>
-          <t>%7B%3EFf</t>
-        </is>
-      </c>
-      <c r="AH8" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="AI8" t="n">
-        <v>0</v>
       </c>
       <c r="AJ8" t="inlineStr">
         <is>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>71bb8625-d14d-41b5-8a04-475b11876eae</t>
+          <t>05de003a-828f-46b1-ba9c-63df15fb2410</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1991,7 +1991,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2024-07-08T01:58:00.000Z</t>
+          <t>2024-07-17T12:15:00.000Z</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>https://www.notion.so/71bb8625d14d41b58a04475b11876eae</t>
+          <t>https://www.notion.so/05de003a828f46b1ba9c63df15fb2410</t>
         </is>
       </c>
       <c r="J9" t="inlineStr"/>
@@ -2076,7 +2076,7 @@
       </c>
       <c r="Y9" t="inlineStr">
         <is>
-          <t>[{'id': '3d301dfe-6e3d-4d28-a249-1fd5fac9abd3'}]</t>
+          <t>[{'id': 'f973382b-037a-4eb1-84bc-e9e5318184b8'}]</t>
         </is>
       </c>
       <c r="Z9" t="b">
@@ -2093,7 +2093,7 @@
         </is>
       </c>
       <c r="AC9" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AD9" t="inlineStr">
         <is>
@@ -2106,7 +2106,7 @@
         </is>
       </c>
       <c r="AF9" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AG9" t="inlineStr">
         <is>
@@ -2119,7 +2119,7 @@
         </is>
       </c>
       <c r="AI9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ9" t="inlineStr">
         <is>
@@ -2138,7 +2138,7 @@
       </c>
       <c r="AM9" t="inlineStr">
         <is>
-          <t>[{'type': 'select', 'select': {'id': 'VWB;', 'name': 'SÓC TRĂNG', 'color': 'red'}}]</t>
+          <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
         </is>
       </c>
       <c r="AN9" t="inlineStr">
@@ -2170,7 +2170,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>82923c0d-8cf4-4fa1-a3b5-52255c0fbc91</t>
+          <t>1cf1ba2b-e08a-4452-b208-684506d74f54</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -2180,7 +2180,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2024-07-08T01:58:00.000Z</t>
+          <t>2024-07-17T12:15:00.000Z</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -2193,7 +2193,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>https://www.notion.so/82923c0d8cf44fa1a3b552255c0fbc91</t>
+          <t>https://www.notion.so/1cf1ba2be08a4452b208684506d74f54</t>
         </is>
       </c>
       <c r="J10" t="inlineStr"/>
@@ -2238,7 +2238,7 @@
         </is>
       </c>
       <c r="S10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T10" t="inlineStr">
         <is>
@@ -2265,7 +2265,7 @@
       </c>
       <c r="Y10" t="inlineStr">
         <is>
-          <t>[{'id': 'a73ea60d-3de1-4e9b-aa7b-f22fda5742bd'}]</t>
+          <t>[{'id': '3fac4a49-402c-4d34-aa91-419ebc20760c'}]</t>
         </is>
       </c>
       <c r="Z10" t="b">
@@ -2282,7 +2282,7 @@
         </is>
       </c>
       <c r="AC10" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="AD10" t="inlineStr">
         <is>
@@ -2295,7 +2295,7 @@
         </is>
       </c>
       <c r="AF10" t="n">
-        <v>6.5</v>
+        <v>14</v>
       </c>
       <c r="AG10" t="inlineStr">
         <is>
@@ -2308,7 +2308,7 @@
         </is>
       </c>
       <c r="AI10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ10" t="inlineStr">
         <is>
@@ -2327,7 +2327,7 @@
       </c>
       <c r="AM10" t="inlineStr">
         <is>
-          <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
+          <t>[{'type': 'select', 'select': {'id': 'VWB;', 'name': 'SÓC TRĂNG', 'color': 'red'}}]</t>
         </is>
       </c>
       <c r="AN10" t="inlineStr">
@@ -2359,7 +2359,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>8838c6b8-138d-4a51-b94c-a61e43096f82</t>
+          <t>dda0b264-3b1d-46ab-85d8-06a4ac6fc467</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2024-07-08T01:58:00.000Z</t>
+          <t>2024-07-17T12:15:00.000Z</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -2382,7 +2382,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>https://www.notion.so/8838c6b8138d4a51b94ca61e43096f82</t>
+          <t>https://www.notion.so/dda0b2643b1d46ab85d806a4ac6fc467</t>
         </is>
       </c>
       <c r="J11" t="inlineStr"/>
@@ -2427,7 +2427,7 @@
         </is>
       </c>
       <c r="S11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11" t="inlineStr">
         <is>
@@ -2454,7 +2454,7 @@
       </c>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>[{'id': '3601e7b0-a80d-4dfd-bfa1-0d34a0e7e389'}]</t>
+          <t>[{'id': '75046948-a198-4627-89b3-3bbf5967526b'}]</t>
         </is>
       </c>
       <c r="Z11" t="b">
@@ -2471,7 +2471,7 @@
         </is>
       </c>
       <c r="AC11" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="AD11" t="inlineStr">
         <is>
@@ -2484,7 +2484,7 @@
         </is>
       </c>
       <c r="AF11" t="n">
-        <v>7</v>
+        <v>18.5</v>
       </c>
       <c r="AG11" t="inlineStr">
         <is>
@@ -2497,7 +2497,7 @@
         </is>
       </c>
       <c r="AI11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ11" t="inlineStr">
         <is>
@@ -2516,7 +2516,7 @@
       </c>
       <c r="AM11" t="inlineStr">
         <is>
-          <t>[{'type': 'select', 'select': {'id': 'Lj_l', 'name': 'LONG XUYÊN', 'color': 'green'}}]</t>
+          <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
         </is>
       </c>
       <c r="AN11" t="inlineStr">
@@ -2548,7 +2548,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ce5aa8e2-193e-4cfb-85c8-d1f2bb956fbc</t>
+          <t>36015951-56f5-48c6-b457-456fdded4f32</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -2558,7 +2558,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2024-07-08T01:58:00.000Z</t>
+          <t>2024-07-17T12:15:00.000Z</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -2571,7 +2571,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>https://www.notion.so/ce5aa8e2193e4cfb85c8d1f2bb956fbc</t>
+          <t>https://www.notion.so/3601595156f548c6b457456fdded4f32</t>
         </is>
       </c>
       <c r="J12" t="inlineStr"/>
@@ -2643,7 +2643,7 @@
       </c>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>[{'id': 'b9c67786-5d99-45c1-85d7-f96bfb66ef22'}]</t>
+          <t>[{'id': 'e49d0ce3-124d-4e4b-b377-be2139cde3f5'}]</t>
         </is>
       </c>
       <c r="Z12" t="b">
@@ -2660,7 +2660,7 @@
         </is>
       </c>
       <c r="AC12" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="AD12" t="inlineStr">
         <is>
@@ -2673,7 +2673,7 @@
         </is>
       </c>
       <c r="AF12" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="AG12" t="inlineStr">
         <is>
@@ -2686,7 +2686,7 @@
         </is>
       </c>
       <c r="AI12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ12" t="inlineStr">
         <is>
@@ -2737,7 +2737,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>d482bb7f-6b24-4f14-958b-0282197809bf</t>
+          <t>48a1d5d5-449f-4119-b338-1f7d4ea3464f</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -2747,7 +2747,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2024-07-08T01:58:00.000Z</t>
+          <t>2024-07-17T12:16:00.000Z</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -2760,7 +2760,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>https://www.notion.so/d482bb7f6b244f14958b0282197809bf</t>
+          <t>https://www.notion.so/48a1d5d5449f4119b3381f7d4ea3464f</t>
         </is>
       </c>
       <c r="J13" t="inlineStr"/>
@@ -2832,7 +2832,7 @@
       </c>
       <c r="Y13" t="inlineStr">
         <is>
-          <t>[{'id': '467f676f-8f46-49b5-afea-feecb0794d23'}]</t>
+          <t>[{'id': 'c463b1a9-4fb2-4258-87a7-44193ba02405'}]</t>
         </is>
       </c>
       <c r="Z13" t="b">
@@ -2849,7 +2849,7 @@
         </is>
       </c>
       <c r="AC13" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="AD13" t="inlineStr">
         <is>
@@ -2862,7 +2862,7 @@
         </is>
       </c>
       <c r="AF13" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="AG13" t="inlineStr">
         <is>
@@ -2894,7 +2894,7 @@
       </c>
       <c r="AM13" t="inlineStr">
         <is>
-          <t>[{'type': 'select', 'select': {'id': 'Lj_l', 'name': 'LONG XUYÊN', 'color': 'green'}}]</t>
+          <t>[{'type': 'select', 'select': {'id': 'VWB;', 'name': 'SÓC TRĂNG', 'color': 'red'}}]</t>
         </is>
       </c>
       <c r="AN13" t="inlineStr">
@@ -2926,7 +2926,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>f16ce82e-4786-421e-a21c-3d6a57cbc51d</t>
+          <t>4a2d1406-11a9-4e3c-80ff-0b01e9355c9b</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -2936,7 +2936,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2024-07-08T01:58:00.000Z</t>
+          <t>2024-07-17T12:16:00.000Z</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -2949,7 +2949,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>https://www.notion.so/f16ce82e4786421ea21c3d6a57cbc51d</t>
+          <t>https://www.notion.so/4a2d140611a94e3c80ff0b01e9355c9b</t>
         </is>
       </c>
       <c r="J14" t="inlineStr"/>
@@ -2994,7 +2994,7 @@
         </is>
       </c>
       <c r="S14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T14" t="inlineStr">
         <is>
@@ -3021,87 +3021,1221 @@
       </c>
       <c r="Y14" t="inlineStr">
         <is>
+          <t>[{'id': 'e926d62c-e624-4663-9009-c562ae5166cf'}]</t>
+        </is>
+      </c>
+      <c r="Z14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA14" t="inlineStr">
+        <is>
+          <t>avzr</t>
+        </is>
+      </c>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AC14" t="n">
+        <v>16</v>
+      </c>
+      <c r="AD14" t="inlineStr">
+        <is>
+          <t>rCIq</t>
+        </is>
+      </c>
+      <c r="AE14" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AF14" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="AG14" t="inlineStr">
+        <is>
+          <t>%7B%3EFf</t>
+        </is>
+      </c>
+      <c r="AH14" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AI14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ14" t="inlineStr">
+        <is>
+          <t>%7BVCZ</t>
+        </is>
+      </c>
+      <c r="AK14" t="inlineStr">
+        <is>
+          <t>rollup</t>
+        </is>
+      </c>
+      <c r="AL14" t="inlineStr">
+        <is>
+          <t>array</t>
+        </is>
+      </c>
+      <c r="AM14" t="inlineStr">
+        <is>
+          <t>[{'type': 'select', 'select': {'id': 'Lj_l', 'name': 'LONG XUYÊN', 'color': 'green'}}]</t>
+        </is>
+      </c>
+      <c r="AN14" t="inlineStr">
+        <is>
+          <t>show_original</t>
+        </is>
+      </c>
+      <c r="AO14" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AP14" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AQ14" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>page</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>71bb8625-d14d-41b5-8a04-475b11876eae</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2024-07-02T18:08:00.000Z</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2024-07-17T12:16:00.000Z</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>https://www.notion.so/71bb8625d14d41b58a04475b11876eae</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>532a166e-c2d9-42ff-bed3-a363f43543fb</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>41cabcaf-915d-46a5-8eff-38727be27269</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>0c70fa05-7bda-4cee-a9f2-3ccf963208ff</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>%3CJjN</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="S15" t="n">
+        <v>2</v>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>%3CK%3FH</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="V15" t="n">
+        <v>0</v>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>Kfrh</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>relation</t>
+        </is>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>[{'id': '3d301dfe-6e3d-4d28-a249-1fd5fac9abd3'}]</t>
+        </is>
+      </c>
+      <c r="Z15" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>avzr</t>
+        </is>
+      </c>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AC15" t="n">
+        <v>12</v>
+      </c>
+      <c r="AD15" t="inlineStr">
+        <is>
+          <t>rCIq</t>
+        </is>
+      </c>
+      <c r="AE15" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AF15" t="n">
+        <v>13</v>
+      </c>
+      <c r="AG15" t="inlineStr">
+        <is>
+          <t>%7B%3EFf</t>
+        </is>
+      </c>
+      <c r="AH15" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AI15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ15" t="inlineStr">
+        <is>
+          <t>%7BVCZ</t>
+        </is>
+      </c>
+      <c r="AK15" t="inlineStr">
+        <is>
+          <t>rollup</t>
+        </is>
+      </c>
+      <c r="AL15" t="inlineStr">
+        <is>
+          <t>array</t>
+        </is>
+      </c>
+      <c r="AM15" t="inlineStr">
+        <is>
+          <t>[{'type': 'select', 'select': {'id': 'VWB;', 'name': 'SÓC TRĂNG', 'color': 'red'}}]</t>
+        </is>
+      </c>
+      <c r="AN15" t="inlineStr">
+        <is>
+          <t>show_original</t>
+        </is>
+      </c>
+      <c r="AO15" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AP15" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AQ15" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>page</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>82923c0d-8cf4-4fa1-a3b5-52255c0fbc91</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2024-07-02T18:08:00.000Z</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2024-07-17T12:16:00.000Z</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>https://www.notion.so/82923c0d8cf44fa1a3b552255c0fbc91</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>532a166e-c2d9-42ff-bed3-a363f43543fb</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>41cabcaf-915d-46a5-8eff-38727be27269</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>0c70fa05-7bda-4cee-a9f2-3ccf963208ff</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>%3CJjN</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="S16" t="n">
+        <v>2</v>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>%3CK%3FH</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="V16" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>Kfrh</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>relation</t>
+        </is>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>[{'id': 'a73ea60d-3de1-4e9b-aa7b-f22fda5742bd'}]</t>
+        </is>
+      </c>
+      <c r="Z16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>avzr</t>
+        </is>
+      </c>
+      <c r="AB16" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AC16" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD16" t="inlineStr">
+        <is>
+          <t>rCIq</t>
+        </is>
+      </c>
+      <c r="AE16" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AF16" t="n">
+        <v>15</v>
+      </c>
+      <c r="AG16" t="inlineStr">
+        <is>
+          <t>%7B%3EFf</t>
+        </is>
+      </c>
+      <c r="AH16" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AI16" t="n">
+        <v>4</v>
+      </c>
+      <c r="AJ16" t="inlineStr">
+        <is>
+          <t>%7BVCZ</t>
+        </is>
+      </c>
+      <c r="AK16" t="inlineStr">
+        <is>
+          <t>rollup</t>
+        </is>
+      </c>
+      <c r="AL16" t="inlineStr">
+        <is>
+          <t>array</t>
+        </is>
+      </c>
+      <c r="AM16" t="inlineStr">
+        <is>
+          <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
+        </is>
+      </c>
+      <c r="AN16" t="inlineStr">
+        <is>
+          <t>show_original</t>
+        </is>
+      </c>
+      <c r="AO16" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AP16" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AQ16" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>page</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>8838c6b8-138d-4a51-b94c-a61e43096f82</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2024-07-02T18:08:00.000Z</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2024-07-17T12:16:00.000Z</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>https://www.notion.so/8838c6b8138d4a51b94ca61e43096f82</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>532a166e-c2d9-42ff-bed3-a363f43543fb</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>41cabcaf-915d-46a5-8eff-38727be27269</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>0c70fa05-7bda-4cee-a9f2-3ccf963208ff</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>%3CJjN</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="S17" t="n">
+        <v>1</v>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>%3CK%3FH</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="V17" t="n">
+        <v>0</v>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>Kfrh</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>relation</t>
+        </is>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>[{'id': '3601e7b0-a80d-4dfd-bfa1-0d34a0e7e389'}]</t>
+        </is>
+      </c>
+      <c r="Z17" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>avzr</t>
+        </is>
+      </c>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AC17" t="n">
+        <v>16</v>
+      </c>
+      <c r="AD17" t="inlineStr">
+        <is>
+          <t>rCIq</t>
+        </is>
+      </c>
+      <c r="AE17" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AF17" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="AG17" t="inlineStr">
+        <is>
+          <t>%7B%3EFf</t>
+        </is>
+      </c>
+      <c r="AH17" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AI17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ17" t="inlineStr">
+        <is>
+          <t>%7BVCZ</t>
+        </is>
+      </c>
+      <c r="AK17" t="inlineStr">
+        <is>
+          <t>rollup</t>
+        </is>
+      </c>
+      <c r="AL17" t="inlineStr">
+        <is>
+          <t>array</t>
+        </is>
+      </c>
+      <c r="AM17" t="inlineStr">
+        <is>
+          <t>[{'type': 'select', 'select': {'id': 'Lj_l', 'name': 'LONG XUYÊN', 'color': 'green'}}]</t>
+        </is>
+      </c>
+      <c r="AN17" t="inlineStr">
+        <is>
+          <t>show_original</t>
+        </is>
+      </c>
+      <c r="AO17" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AP17" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AQ17" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>page</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ce5aa8e2-193e-4cfb-85c8-d1f2bb956fbc</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2024-07-02T18:08:00.000Z</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2024-07-17T12:16:00.000Z</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>https://www.notion.so/ce5aa8e2193e4cfb85c8d1f2bb956fbc</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>532a166e-c2d9-42ff-bed3-a363f43543fb</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>41cabcaf-915d-46a5-8eff-38727be27269</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>0c70fa05-7bda-4cee-a9f2-3ccf963208ff</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>%3CJjN</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="S18" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>%3CK%3FH</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="V18" t="n">
+        <v>0</v>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>Kfrh</t>
+        </is>
+      </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>relation</t>
+        </is>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>[{'id': 'b9c67786-5d99-45c1-85d7-f96bfb66ef22'}]</t>
+        </is>
+      </c>
+      <c r="Z18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>avzr</t>
+        </is>
+      </c>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AC18" t="n">
+        <v>16</v>
+      </c>
+      <c r="AD18" t="inlineStr">
+        <is>
+          <t>rCIq</t>
+        </is>
+      </c>
+      <c r="AE18" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AF18" t="n">
+        <v>16</v>
+      </c>
+      <c r="AG18" t="inlineStr">
+        <is>
+          <t>%7B%3EFf</t>
+        </is>
+      </c>
+      <c r="AH18" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AI18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ18" t="inlineStr">
+        <is>
+          <t>%7BVCZ</t>
+        </is>
+      </c>
+      <c r="AK18" t="inlineStr">
+        <is>
+          <t>rollup</t>
+        </is>
+      </c>
+      <c r="AL18" t="inlineStr">
+        <is>
+          <t>array</t>
+        </is>
+      </c>
+      <c r="AM18" t="inlineStr">
+        <is>
+          <t>[{'type': 'select', 'select': {'id': 'KqT_', 'name': 'CẦN THƠ', 'color': 'purple'}}]</t>
+        </is>
+      </c>
+      <c r="AN18" t="inlineStr">
+        <is>
+          <t>show_original</t>
+        </is>
+      </c>
+      <c r="AO18" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AP18" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AQ18" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>page</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>d482bb7f-6b24-4f14-958b-0282197809bf</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2024-07-02T18:08:00.000Z</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2024-07-17T12:16:00.000Z</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>https://www.notion.so/d482bb7f6b244f14958b0282197809bf</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>532a166e-c2d9-42ff-bed3-a363f43543fb</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>41cabcaf-915d-46a5-8eff-38727be27269</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>0c70fa05-7bda-4cee-a9f2-3ccf963208ff</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>%3CJjN</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>%3CK%3FH</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="V19" t="n">
+        <v>0</v>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>Kfrh</t>
+        </is>
+      </c>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>relation</t>
+        </is>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>[{'id': '467f676f-8f46-49b5-afea-feecb0794d23'}]</t>
+        </is>
+      </c>
+      <c r="Z19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>avzr</t>
+        </is>
+      </c>
+      <c r="AB19" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AC19" t="n">
+        <v>16</v>
+      </c>
+      <c r="AD19" t="inlineStr">
+        <is>
+          <t>rCIq</t>
+        </is>
+      </c>
+      <c r="AE19" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AF19" t="n">
+        <v>17</v>
+      </c>
+      <c r="AG19" t="inlineStr">
+        <is>
+          <t>%7B%3EFf</t>
+        </is>
+      </c>
+      <c r="AH19" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AI19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ19" t="inlineStr">
+        <is>
+          <t>%7BVCZ</t>
+        </is>
+      </c>
+      <c r="AK19" t="inlineStr">
+        <is>
+          <t>rollup</t>
+        </is>
+      </c>
+      <c r="AL19" t="inlineStr">
+        <is>
+          <t>array</t>
+        </is>
+      </c>
+      <c r="AM19" t="inlineStr">
+        <is>
+          <t>[{'type': 'select', 'select': {'id': 'Lj_l', 'name': 'LONG XUYÊN', 'color': 'green'}}]</t>
+        </is>
+      </c>
+      <c r="AN19" t="inlineStr">
+        <is>
+          <t>show_original</t>
+        </is>
+      </c>
+      <c r="AO19" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AP19" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="AQ19" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>page</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>f16ce82e-4786-421e-a21c-3d6a57cbc51d</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2024-07-02T18:08:00.000Z</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2024-07-17T12:16:00.000Z</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>https://www.notion.so/f16ce82e4786421ea21c3d6a57cbc51d</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>532a166e-c2d9-42ff-bed3-a363f43543fb</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>user</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>41cabcaf-915d-46a5-8eff-38727be27269</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>0c70fa05-7bda-4cee-a9f2-3ccf963208ff</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>%3CJjN</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="S20" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>%3CK%3FH</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="V20" t="n">
+        <v>0</v>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>Kfrh</t>
+        </is>
+      </c>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>relation</t>
+        </is>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
           <t>[{'id': 'd1ae645f-f3dd-46cd-a715-a8c150605da6'}]</t>
         </is>
       </c>
-      <c r="Z14" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA14" t="inlineStr">
+      <c r="Z20" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA20" t="inlineStr">
         <is>
           <t>avzr</t>
         </is>
       </c>
-      <c r="AB14" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="AC14" t="n">
-        <v>7</v>
-      </c>
-      <c r="AD14" t="inlineStr">
+      <c r="AB20" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AC20" t="n">
+        <v>17</v>
+      </c>
+      <c r="AD20" t="inlineStr">
         <is>
           <t>rCIq</t>
         </is>
       </c>
-      <c r="AE14" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="AF14" t="n">
-        <v>7</v>
-      </c>
-      <c r="AG14" t="inlineStr">
+      <c r="AE20" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AF20" t="n">
+        <v>17</v>
+      </c>
+      <c r="AG20" t="inlineStr">
         <is>
           <t>%7B%3EFf</t>
         </is>
       </c>
-      <c r="AH14" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="AI14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ14" t="inlineStr">
+      <c r="AH20" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="AI20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ20" t="inlineStr">
         <is>
           <t>%7BVCZ</t>
         </is>
       </c>
-      <c r="AK14" t="inlineStr">
+      <c r="AK20" t="inlineStr">
         <is>
           <t>rollup</t>
         </is>
       </c>
-      <c r="AL14" t="inlineStr">
+      <c r="AL20" t="inlineStr">
         <is>
           <t>array</t>
         </is>
       </c>
-      <c r="AM14" t="inlineStr">
+      <c r="AM20" t="inlineStr">
         <is>
           <t>[{'type': 'select', 'select': {'id': 'Lj_l', 'name': 'LONG XUYÊN', 'color': 'green'}}]</t>
         </is>
       </c>
-      <c r="AN14" t="inlineStr">
+      <c r="AN20" t="inlineStr">
         <is>
           <t>show_original</t>
         </is>
       </c>
-      <c r="AO14" t="inlineStr">
+      <c r="AO20" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AP14" t="inlineStr">
+      <c r="AP20" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="AQ14" t="inlineStr">
+      <c r="AQ20" t="inlineStr">
         <is>
           <t>[]</t>
         </is>

</xml_diff>

<commit_message>
Update code tinh luong % format cac bang
</commit_message>
<xml_diff>
--- a/notion_data/CHAM_CONG_HE_THONG.xlsx
+++ b/notion_data/CHAM_CONG_HE_THONG.xlsx
@@ -668,7 +668,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-07-17T17:23:00.000Z</t>
+          <t>2024-07-18T15:58:00.000Z</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -770,7 +770,7 @@
         </is>
       </c>
       <c r="AC2" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AD2" t="inlineStr">
         <is>
@@ -783,7 +783,7 @@
         </is>
       </c>
       <c r="AF2" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AG2" t="inlineStr">
         <is>
@@ -857,7 +857,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2024-07-17T17:23:00.000Z</t>
+          <t>2024-07-18T15:58:00.000Z</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -959,7 +959,7 @@
         </is>
       </c>
       <c r="AC3" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AD3" t="inlineStr">
         <is>
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="AF3" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AG3" t="inlineStr">
         <is>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2024-07-17T17:23:00.000Z</t>
+          <t>2024-07-18T15:58:00.000Z</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2024-07-17T17:23:00.000Z</t>
+          <t>2024-07-18T15:58:00.000Z</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -1424,7 +1424,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2024-07-17T17:23:00.000Z</t>
+          <t>2024-07-18T15:58:00.000Z</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -1526,7 +1526,7 @@
         </is>
       </c>
       <c r="AC6" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AD6" t="inlineStr">
         <is>
@@ -1539,7 +1539,7 @@
         </is>
       </c>
       <c r="AF6" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AG6" t="inlineStr">
         <is>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2024-07-17T17:23:00.000Z</t>
+          <t>2024-07-18T15:58:00.000Z</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="AC7" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AD7" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
         </is>
       </c>
       <c r="AF7" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AG7" t="inlineStr">
         <is>
@@ -1802,7 +1802,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2024-07-17T17:23:00.000Z</t>
+          <t>2024-07-18T15:58:00.000Z</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -1904,7 +1904,7 @@
         </is>
       </c>
       <c r="AC8" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AD8" t="inlineStr">
         <is>
@@ -1917,7 +1917,7 @@
         </is>
       </c>
       <c r="AF8" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AG8" t="inlineStr">
         <is>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2024-07-17T17:23:00.000Z</t>
+          <t>2024-07-18T15:58:00.000Z</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -2093,7 +2093,7 @@
         </is>
       </c>
       <c r="AC9" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AD9" t="inlineStr">
         <is>
@@ -2106,7 +2106,7 @@
         </is>
       </c>
       <c r="AF9" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AG9" t="inlineStr">
         <is>
@@ -2180,7 +2180,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2024-07-17T17:23:00.000Z</t>
+          <t>2024-07-18T15:58:00.000Z</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2024-07-17T17:23:00.000Z</t>
+          <t>2024-07-18T15:58:00.000Z</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -2471,7 +2471,7 @@
         </is>
       </c>
       <c r="AC11" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AD11" t="inlineStr">
         <is>
@@ -2484,7 +2484,7 @@
         </is>
       </c>
       <c r="AF11" t="n">
-        <v>18.5</v>
+        <v>19.5</v>
       </c>
       <c r="AG11" t="inlineStr">
         <is>
@@ -2558,7 +2558,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2024-07-17T17:23:00.000Z</t>
+          <t>2024-07-18T15:58:00.000Z</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -2660,7 +2660,7 @@
         </is>
       </c>
       <c r="AC12" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AD12" t="inlineStr">
         <is>
@@ -2673,7 +2673,7 @@
         </is>
       </c>
       <c r="AF12" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AG12" t="inlineStr">
         <is>
@@ -2747,7 +2747,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2024-07-17T17:23:00.000Z</t>
+          <t>2024-07-18T15:58:00.000Z</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -2936,7 +2936,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2024-07-17T17:23:00.000Z</t>
+          <t>2024-07-18T15:58:00.000Z</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -3038,7 +3038,7 @@
         </is>
       </c>
       <c r="AC14" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AD14" t="inlineStr">
         <is>
@@ -3051,7 +3051,7 @@
         </is>
       </c>
       <c r="AF14" t="n">
-        <v>16.5</v>
+        <v>17.5</v>
       </c>
       <c r="AG14" t="inlineStr">
         <is>
@@ -3125,7 +3125,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2024-07-17T17:24:00.000Z</t>
+          <t>2024-07-18T15:58:00.000Z</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -3314,7 +3314,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2024-07-17T17:24:00.000Z</t>
+          <t>2024-07-18T15:58:00.000Z</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -3416,7 +3416,7 @@
         </is>
       </c>
       <c r="AC16" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AD16" t="inlineStr">
         <is>
@@ -3429,7 +3429,7 @@
         </is>
       </c>
       <c r="AF16" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AG16" t="inlineStr">
         <is>
@@ -3503,7 +3503,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2024-07-17T17:24:00.000Z</t>
+          <t>2024-07-18T15:58:00.000Z</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -3605,7 +3605,7 @@
         </is>
       </c>
       <c r="AC17" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AD17" t="inlineStr">
         <is>
@@ -3618,7 +3618,7 @@
         </is>
       </c>
       <c r="AF17" t="n">
-        <v>16.5</v>
+        <v>17.5</v>
       </c>
       <c r="AG17" t="inlineStr">
         <is>
@@ -3692,7 +3692,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2024-07-17T17:24:00.000Z</t>
+          <t>2024-07-18T15:58:00.000Z</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -3794,7 +3794,7 @@
         </is>
       </c>
       <c r="AC18" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AD18" t="inlineStr">
         <is>
@@ -3807,7 +3807,7 @@
         </is>
       </c>
       <c r="AF18" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AG18" t="inlineStr">
         <is>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2024-07-17T17:24:00.000Z</t>
+          <t>2024-07-18T15:58:00.000Z</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -3983,7 +3983,7 @@
         </is>
       </c>
       <c r="AC19" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AD19" t="inlineStr">
         <is>
@@ -3996,7 +3996,7 @@
         </is>
       </c>
       <c r="AF19" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AG19" t="inlineStr">
         <is>
@@ -4070,7 +4070,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2024-07-17T17:24:00.000Z</t>
+          <t>2024-07-18T15:58:00.000Z</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -4172,7 +4172,7 @@
         </is>
       </c>
       <c r="AC20" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AD20" t="inlineStr">
         <is>
@@ -4185,7 +4185,7 @@
         </is>
       </c>
       <c r="AF20" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AG20" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
code 2 truong hop dac bien của Quyen và anh Hau
</commit_message>
<xml_diff>
--- a/notion_data/CHAM_CONG_HE_THONG.xlsx
+++ b/notion_data/CHAM_CONG_HE_THONG.xlsx
@@ -668,7 +668,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-07-18T15:58:00.000Z</t>
+          <t>2024-07-19T08:01:00.000Z</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -857,7 +857,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2024-07-18T15:58:00.000Z</t>
+          <t>2024-07-19T08:01:00.000Z</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2024-07-18T15:58:00.000Z</t>
+          <t>2024-07-19T08:01:00.000Z</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2024-07-18T15:58:00.000Z</t>
+          <t>2024-07-19T08:01:00.000Z</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -1424,7 +1424,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2024-07-18T15:58:00.000Z</t>
+          <t>2024-07-19T08:01:00.000Z</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2024-07-18T15:58:00.000Z</t>
+          <t>2024-07-19T08:01:00.000Z</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -1802,7 +1802,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2024-07-18T15:58:00.000Z</t>
+          <t>2024-07-19T08:01:00.000Z</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2024-07-18T15:58:00.000Z</t>
+          <t>2024-07-19T08:01:00.000Z</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -2180,7 +2180,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2024-07-18T15:58:00.000Z</t>
+          <t>2024-07-19T08:01:00.000Z</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2024-07-18T15:58:00.000Z</t>
+          <t>2024-07-19T08:01:00.000Z</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -2558,7 +2558,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2024-07-18T15:58:00.000Z</t>
+          <t>2024-07-19T08:01:00.000Z</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -2747,7 +2747,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2024-07-18T15:58:00.000Z</t>
+          <t>2024-07-19T08:01:00.000Z</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -2936,7 +2936,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2024-07-18T15:58:00.000Z</t>
+          <t>2024-07-19T08:01:00.000Z</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -3125,7 +3125,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2024-07-18T15:58:00.000Z</t>
+          <t>2024-07-19T08:01:00.000Z</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -3314,7 +3314,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2024-07-18T15:58:00.000Z</t>
+          <t>2024-07-19T08:01:00.000Z</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -3503,7 +3503,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2024-07-18T15:58:00.000Z</t>
+          <t>2024-07-19T08:01:00.000Z</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -3692,7 +3692,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2024-07-18T15:58:00.000Z</t>
+          <t>2024-07-19T08:01:00.000Z</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2024-07-18T15:58:00.000Z</t>
+          <t>2024-07-19T08:01:00.000Z</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -4070,7 +4070,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2024-07-18T15:58:00.000Z</t>
+          <t>2024-07-19T08:01:00.000Z</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>

</xml_diff>

<commit_message>
update code tinh luong cho Quyen
</commit_message>
<xml_diff>
--- a/notion_data/CHAM_CONG_HE_THONG.xlsx
+++ b/notion_data/CHAM_CONG_HE_THONG.xlsx
@@ -668,7 +668,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-07-19T08:01:00.000Z</t>
+          <t>2024-07-19T12:51:00.000Z</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -770,7 +770,7 @@
         </is>
       </c>
       <c r="AC2" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AD2" t="inlineStr">
         <is>
@@ -783,7 +783,7 @@
         </is>
       </c>
       <c r="AF2" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AG2" t="inlineStr">
         <is>
@@ -857,7 +857,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2024-07-19T08:01:00.000Z</t>
+          <t>2024-07-19T12:51:00.000Z</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -959,7 +959,7 @@
         </is>
       </c>
       <c r="AC3" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AD3" t="inlineStr">
         <is>
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="AF3" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AG3" t="inlineStr">
         <is>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2024-07-19T08:01:00.000Z</t>
+          <t>2024-07-19T12:51:00.000Z</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -1148,7 +1148,7 @@
         </is>
       </c>
       <c r="AC4" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="AD4" t="inlineStr">
         <is>
@@ -1161,7 +1161,7 @@
         </is>
       </c>
       <c r="AF4" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="AG4" t="inlineStr">
         <is>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2024-07-19T08:01:00.000Z</t>
+          <t>2024-07-19T12:51:00.000Z</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -1424,7 +1424,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2024-07-19T08:01:00.000Z</t>
+          <t>2024-07-19T12:51:00.000Z</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -1526,7 +1526,7 @@
         </is>
       </c>
       <c r="AC6" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AD6" t="inlineStr">
         <is>
@@ -1539,7 +1539,7 @@
         </is>
       </c>
       <c r="AF6" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AG6" t="inlineStr">
         <is>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2024-07-19T08:01:00.000Z</t>
+          <t>2024-07-19T12:51:00.000Z</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="AC7" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AD7" t="inlineStr">
         <is>
@@ -1728,7 +1728,7 @@
         </is>
       </c>
       <c r="AF7" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AG7" t="inlineStr">
         <is>
@@ -1802,7 +1802,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2024-07-19T08:01:00.000Z</t>
+          <t>2024-07-19T12:51:00.000Z</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2024-07-19T08:01:00.000Z</t>
+          <t>2024-07-19T12:51:00.000Z</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -2093,7 +2093,7 @@
         </is>
       </c>
       <c r="AC9" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AD9" t="inlineStr">
         <is>
@@ -2106,7 +2106,7 @@
         </is>
       </c>
       <c r="AF9" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AG9" t="inlineStr">
         <is>
@@ -2180,7 +2180,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2024-07-19T08:01:00.000Z</t>
+          <t>2024-07-19T12:52:00.000Z</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -2282,7 +2282,7 @@
         </is>
       </c>
       <c r="AC10" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="AD10" t="inlineStr">
         <is>
@@ -2295,7 +2295,7 @@
         </is>
       </c>
       <c r="AF10" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="AG10" t="inlineStr">
         <is>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2024-07-19T08:01:00.000Z</t>
+          <t>2024-07-19T12:52:00.000Z</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -2427,7 +2427,7 @@
         </is>
       </c>
       <c r="S11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T11" t="inlineStr">
         <is>
@@ -2471,7 +2471,7 @@
         </is>
       </c>
       <c r="AC11" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AD11" t="inlineStr">
         <is>
@@ -2484,7 +2484,7 @@
         </is>
       </c>
       <c r="AF11" t="n">
-        <v>19.5</v>
+        <v>21</v>
       </c>
       <c r="AG11" t="inlineStr">
         <is>
@@ -2558,7 +2558,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2024-07-19T08:01:00.000Z</t>
+          <t>2024-07-19T12:52:00.000Z</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -2660,7 +2660,7 @@
         </is>
       </c>
       <c r="AC12" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AD12" t="inlineStr">
         <is>
@@ -2673,7 +2673,7 @@
         </is>
       </c>
       <c r="AF12" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AG12" t="inlineStr">
         <is>
@@ -2747,7 +2747,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2024-07-19T08:01:00.000Z</t>
+          <t>2024-07-19T12:52:00.000Z</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -2849,7 +2849,7 @@
         </is>
       </c>
       <c r="AC13" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="AD13" t="inlineStr">
         <is>
@@ -2862,7 +2862,7 @@
         </is>
       </c>
       <c r="AF13" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="AG13" t="inlineStr">
         <is>
@@ -2936,7 +2936,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2024-07-19T08:01:00.000Z</t>
+          <t>2024-07-19T12:52:00.000Z</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -3125,7 +3125,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2024-07-19T08:01:00.000Z</t>
+          <t>2024-07-19T12:52:00.000Z</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -3227,7 +3227,7 @@
         </is>
       </c>
       <c r="AC15" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="AD15" t="inlineStr">
         <is>
@@ -3240,7 +3240,7 @@
         </is>
       </c>
       <c r="AF15" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="AG15" t="inlineStr">
         <is>
@@ -3314,7 +3314,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2024-07-19T08:01:00.000Z</t>
+          <t>2024-07-19T12:52:00.000Z</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -3416,7 +3416,7 @@
         </is>
       </c>
       <c r="AC16" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AD16" t="inlineStr">
         <is>
@@ -3429,7 +3429,7 @@
         </is>
       </c>
       <c r="AF16" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AG16" t="inlineStr">
         <is>
@@ -3503,7 +3503,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2024-07-19T08:01:00.000Z</t>
+          <t>2024-07-19T12:52:00.000Z</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -3692,7 +3692,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2024-07-19T08:01:00.000Z</t>
+          <t>2024-07-19T12:52:00.000Z</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -3794,7 +3794,7 @@
         </is>
       </c>
       <c r="AC18" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AD18" t="inlineStr">
         <is>
@@ -3807,7 +3807,7 @@
         </is>
       </c>
       <c r="AF18" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AG18" t="inlineStr">
         <is>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2024-07-19T08:01:00.000Z</t>
+          <t>2024-07-19T12:52:00.000Z</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -4070,7 +4070,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2024-07-19T08:01:00.000Z</t>
+          <t>2024-07-19T12:52:00.000Z</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>

</xml_diff>

<commit_message>
update code vi co su khac nhau giua mac va win
</commit_message>
<xml_diff>
--- a/notion_data/CHAM_CONG_HE_THONG.xlsx
+++ b/notion_data/CHAM_CONG_HE_THONG.xlsx
@@ -668,7 +668,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-07-19T12:51:00.000Z</t>
+          <t>2024-07-20T13:34:00.000Z</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -857,7 +857,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2024-07-19T12:51:00.000Z</t>
+          <t>2024-07-20T13:34:00.000Z</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2024-07-19T12:51:00.000Z</t>
+          <t>2024-07-20T13:34:00.000Z</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2024-07-19T12:51:00.000Z</t>
+          <t>2024-07-20T13:34:00.000Z</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -1424,7 +1424,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2024-07-19T12:51:00.000Z</t>
+          <t>2024-07-20T13:34:00.000Z</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2024-07-19T12:51:00.000Z</t>
+          <t>2024-07-20T13:34:00.000Z</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -1802,7 +1802,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2024-07-19T12:51:00.000Z</t>
+          <t>2024-07-20T13:34:00.000Z</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -1904,7 +1904,7 @@
         </is>
       </c>
       <c r="AC8" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AD8" t="inlineStr">
         <is>
@@ -1917,7 +1917,7 @@
         </is>
       </c>
       <c r="AF8" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AG8" t="inlineStr">
         <is>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2024-07-19T12:51:00.000Z</t>
+          <t>2024-07-20T13:34:00.000Z</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -2180,7 +2180,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2024-07-19T12:52:00.000Z</t>
+          <t>2024-07-20T13:35:00.000Z</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2024-07-19T12:52:00.000Z</t>
+          <t>2024-07-20T13:35:00.000Z</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -2558,7 +2558,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2024-07-19T12:52:00.000Z</t>
+          <t>2024-07-20T13:35:00.000Z</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -2747,7 +2747,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2024-07-19T12:52:00.000Z</t>
+          <t>2024-07-20T13:35:00.000Z</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -2936,7 +2936,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2024-07-19T12:52:00.000Z</t>
+          <t>2024-07-20T13:35:00.000Z</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -3038,7 +3038,7 @@
         </is>
       </c>
       <c r="AC14" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AD14" t="inlineStr">
         <is>
@@ -3051,7 +3051,7 @@
         </is>
       </c>
       <c r="AF14" t="n">
-        <v>17.5</v>
+        <v>18.5</v>
       </c>
       <c r="AG14" t="inlineStr">
         <is>
@@ -3125,7 +3125,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2024-07-19T12:52:00.000Z</t>
+          <t>2024-07-20T13:35:00.000Z</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -3314,7 +3314,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2024-07-19T12:52:00.000Z</t>
+          <t>2024-07-20T13:35:00.000Z</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -3503,7 +3503,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2024-07-19T12:52:00.000Z</t>
+          <t>2024-07-20T13:35:00.000Z</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -3605,7 +3605,7 @@
         </is>
       </c>
       <c r="AC17" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AD17" t="inlineStr">
         <is>
@@ -3618,7 +3618,7 @@
         </is>
       </c>
       <c r="AF17" t="n">
-        <v>17.5</v>
+        <v>18.5</v>
       </c>
       <c r="AG17" t="inlineStr">
         <is>
@@ -3692,7 +3692,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2024-07-19T12:52:00.000Z</t>
+          <t>2024-07-20T13:35:00.000Z</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2024-07-19T12:52:00.000Z</t>
+          <t>2024-07-20T13:35:00.000Z</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -3983,7 +3983,7 @@
         </is>
       </c>
       <c r="AC19" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AD19" t="inlineStr">
         <is>
@@ -3996,7 +3996,7 @@
         </is>
       </c>
       <c r="AF19" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AG19" t="inlineStr">
         <is>
@@ -4070,7 +4070,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2024-07-19T12:52:00.000Z</t>
+          <t>2024-07-20T13:35:00.000Z</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -4172,7 +4172,7 @@
         </is>
       </c>
       <c r="AC20" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AD20" t="inlineStr">
         <is>
@@ -4185,7 +4185,7 @@
         </is>
       </c>
       <c r="AF20" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AG20" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
sua chiet khau cua sale phu va update chien luoc chay tinh luong theo gio
</commit_message>
<xml_diff>
--- a/notion_data/CHAM_CONG_HE_THONG.xlsx
+++ b/notion_data/CHAM_CONG_HE_THONG.xlsx
@@ -668,7 +668,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-07-20T13:34:00.000Z</t>
+          <t>2024-07-21T16:44:00.000Z</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -857,7 +857,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2024-07-20T13:34:00.000Z</t>
+          <t>2024-07-21T16:44:00.000Z</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2024-07-20T13:34:00.000Z</t>
+          <t>2024-07-21T16:44:00.000Z</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2024-07-20T13:34:00.000Z</t>
+          <t>2024-07-21T16:44:00.000Z</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -1424,7 +1424,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2024-07-20T13:34:00.000Z</t>
+          <t>2024-07-21T16:44:00.000Z</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2024-07-20T13:34:00.000Z</t>
+          <t>2024-07-21T16:44:00.000Z</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -1802,7 +1802,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2024-07-20T13:34:00.000Z</t>
+          <t>2024-07-21T16:44:00.000Z</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
@@ -1904,7 +1904,7 @@
         </is>
       </c>
       <c r="AC8" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="AD8" t="inlineStr">
         <is>
@@ -1917,7 +1917,7 @@
         </is>
       </c>
       <c r="AF8" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="AG8" t="inlineStr">
         <is>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2024-07-20T13:34:00.000Z</t>
+          <t>2024-07-21T16:44:00.000Z</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -2180,7 +2180,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2024-07-20T13:35:00.000Z</t>
+          <t>2024-07-21T16:44:00.000Z</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2024-07-20T13:35:00.000Z</t>
+          <t>2024-07-21T16:44:00.000Z</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -2471,7 +2471,7 @@
         </is>
       </c>
       <c r="AC11" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AD11" t="inlineStr">
         <is>
@@ -2484,7 +2484,7 @@
         </is>
       </c>
       <c r="AF11" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AG11" t="inlineStr">
         <is>
@@ -2558,7 +2558,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2024-07-20T13:35:00.000Z</t>
+          <t>2024-07-21T16:44:00.000Z</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -2747,7 +2747,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2024-07-20T13:35:00.000Z</t>
+          <t>2024-07-21T16:44:00.000Z</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -2936,7 +2936,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2024-07-20T13:35:00.000Z</t>
+          <t>2024-07-21T16:44:00.000Z</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -3038,7 +3038,7 @@
         </is>
       </c>
       <c r="AC14" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="AD14" t="inlineStr">
         <is>
@@ -3051,7 +3051,7 @@
         </is>
       </c>
       <c r="AF14" t="n">
-        <v>18.5</v>
+        <v>20.5</v>
       </c>
       <c r="AG14" t="inlineStr">
         <is>
@@ -3125,7 +3125,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2024-07-20T13:35:00.000Z</t>
+          <t>2024-07-21T16:44:00.000Z</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -3314,7 +3314,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2024-07-20T13:35:00.000Z</t>
+          <t>2024-07-21T16:44:00.000Z</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -3503,7 +3503,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2024-07-20T13:35:00.000Z</t>
+          <t>2024-07-21T16:44:00.000Z</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -3605,7 +3605,7 @@
         </is>
       </c>
       <c r="AC17" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="AD17" t="inlineStr">
         <is>
@@ -3618,7 +3618,7 @@
         </is>
       </c>
       <c r="AF17" t="n">
-        <v>18.5</v>
+        <v>20.5</v>
       </c>
       <c r="AG17" t="inlineStr">
         <is>
@@ -3692,7 +3692,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2024-07-20T13:35:00.000Z</t>
+          <t>2024-07-21T16:44:00.000Z</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2024-07-20T13:35:00.000Z</t>
+          <t>2024-07-21T16:44:00.000Z</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -3983,7 +3983,7 @@
         </is>
       </c>
       <c r="AC19" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="AD19" t="inlineStr">
         <is>
@@ -3996,7 +3996,7 @@
         </is>
       </c>
       <c r="AF19" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="AG19" t="inlineStr">
         <is>
@@ -4070,7 +4070,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2024-07-20T13:35:00.000Z</t>
+          <t>2024-07-21T16:44:00.000Z</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -4172,7 +4172,7 @@
         </is>
       </c>
       <c r="AC20" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="AD20" t="inlineStr">
         <is>
@@ -4185,7 +4185,7 @@
         </is>
       </c>
       <c r="AF20" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="AG20" t="inlineStr">
         <is>

</xml_diff>